<commit_message>
Updates on convergence testing.
It looks like Monte Carlo might not work straightforwardly. Maybe can look into tensor network decoding for how to compute information quantities.
</commit_message>
<xml_diff>
--- a/Convergence.xlsx
+++ b/Convergence.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e00c848d2da39f20/Documents/3.Masters/Thesis/Code/MutualInfo/QEC_MI_MonteCarlo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="256" documentId="11_F25DC773A252ABDACC1048BDC11F63425BDE58E3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CC447107-59D0-438C-8FFB-90E9F221B1A8}"/>
+  <xr:revisionPtr revIDLastSave="332" documentId="11_F25DC773A252ABDACC1048BDC11F63425BDE58E3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{05388BDA-CB1E-43DD-A7A6-CCEECD11FB15}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="14">
   <si>
     <t>L=2</t>
   </si>
@@ -72,6 +72,12 @@
   </si>
   <si>
     <t>L=5</t>
+  </si>
+  <si>
+    <t>L=6</t>
+  </si>
+  <si>
+    <t>Number of possible errors</t>
   </si>
 </sst>
 </file>
@@ -195,7 +201,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -205,7 +211,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -303,38 +312,32 @@
           <c:xVal>
             <c:numLit>
               <c:formatCode>General</c:formatCode>
-              <c:ptCount val="4"/>
+              <c:ptCount val="3"/>
               <c:pt idx="0">
                 <c:v>2</c:v>
               </c:pt>
               <c:pt idx="1">
-                <c:v>3</c:v>
+                <c:v>4</c:v>
               </c:pt>
               <c:pt idx="2">
-                <c:v>4</c:v>
-              </c:pt>
-              <c:pt idx="3">
-                <c:v>5</c:v>
+                <c:v>6</c:v>
               </c:pt>
             </c:numLit>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$R$6:$U$6</c:f>
+              <c:f>(Sheet1!$V$6,Sheet1!$X$6,Sheet1!$Z$6)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>0.273615953507439</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.13532506507394701</c:v>
+                  <c:v>0.28627499822907598</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.28627499822907598</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.64546168029639195</c:v>
+                  <c:v>0.83588158006639501</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1094,15 +1097,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>441960</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>140970</xdr:rowOff>
+      <xdr:colOff>396240</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>156210</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>137160</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>140970</xdr:rowOff>
+      <xdr:colOff>91440</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>156210</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1397,476 +1400,624 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U11"/>
+  <dimension ref="A1:Z13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="2" t="s">
+      <c r="E1" s="3"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3"/>
       <c r="H1" s="3"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="2" t="s">
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="2" t="s">
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="R1" s="3"/>
       <c r="S1" s="3"/>
       <c r="T1" s="3"/>
       <c r="U1" s="4"/>
+      <c r="V1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="4"/>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="J2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="K2" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="L2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="O2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="P2" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="O2" t="s">
+      <c r="R2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="P2" t="s">
+      <c r="S2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="T2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="R2" s="5" t="s">
+      <c r="U2" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="V2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="S2" t="s">
+      <c r="W2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="T2" t="s">
+      <c r="X2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="U2" s="6" t="s">
+      <c r="Y2" s="9" t="s">
         <v>11</v>
       </c>
+      <c r="Z2" s="6" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A3">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A3" s="12">
         <f>10^3</f>
         <v>1000</v>
       </c>
       <c r="B3" s="5">
         <v>3.63906932787524</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="9">
         <v>7.35273934818116</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="9">
         <v>9.5504002180521397</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="9">
         <v>9.9242745096576908</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="6">
+        <v>9.9657842846620106</v>
+      </c>
+      <c r="G3" s="5">
         <v>2.4472065907296798</v>
       </c>
-      <c r="G3">
+      <c r="H3" s="9">
         <v>6.6309771114962697</v>
       </c>
-      <c r="H3">
+      <c r="I3" s="9">
         <v>9.4651160055370003</v>
       </c>
-      <c r="I3" s="6">
+      <c r="J3" s="9">
         <v>9.9242745096576908</v>
       </c>
-      <c r="J3" s="5">
+      <c r="K3" s="6">
+        <v>9.9657842846620106</v>
+      </c>
+      <c r="L3" s="5">
         <v>0.93317179842408904</v>
       </c>
-      <c r="K3">
+      <c r="M3" s="9">
         <v>0.75093197963384595</v>
       </c>
-      <c r="L3">
+      <c r="N3" s="9">
         <v>0.86872124633940395</v>
       </c>
-      <c r="M3" s="6">
+      <c r="O3" s="9">
         <v>0.783204430282889</v>
       </c>
-      <c r="N3" s="5">
+      <c r="P3" s="6">
+        <v>0.87129078401035898</v>
+      </c>
+      <c r="Q3" s="5">
         <v>3.0503907781573201</v>
       </c>
-      <c r="O3">
+      <c r="R3" s="9">
         <v>7.0390890884613802</v>
       </c>
-      <c r="P3">
+      <c r="S3" s="9">
         <v>9.5001355555456506</v>
       </c>
-      <c r="Q3" s="6">
+      <c r="T3" s="9">
         <v>9.9242745096576908</v>
       </c>
-      <c r="R3" s="5">
+      <c r="U3" s="6">
+        <v>9.9657842846620106</v>
+      </c>
+      <c r="V3" s="5">
         <v>0.32998761099645002</v>
       </c>
-      <c r="S3">
+      <c r="W3" s="9">
         <v>0.34282000266873702</v>
       </c>
-      <c r="T3">
+      <c r="X3" s="9">
         <v>0.83370169633075197</v>
       </c>
-      <c r="U3" s="6">
+      <c r="Y3" s="9">
         <v>0.783204430282889</v>
       </c>
+      <c r="Z3" s="6">
+        <v>0.87129078401035898</v>
+      </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A4">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A4" s="12">
         <f>10^4</f>
         <v>10000</v>
       </c>
       <c r="B4" s="5">
         <v>3.7649003376452002</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="9">
         <v>8.0198059704979006</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="9">
         <v>11.7721183211632</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="9">
         <v>13.128361893507099</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="6">
+        <v>13.2830717423524</v>
+      </c>
+      <c r="G4" s="5">
         <v>2.4714614641235899</v>
       </c>
-      <c r="G4">
+      <c r="H4" s="9">
         <v>6.6492169278796398</v>
       </c>
-      <c r="H4">
+      <c r="I4" s="9">
         <v>11.3700282942785</v>
       </c>
-      <c r="I4" s="6">
+      <c r="J4" s="9">
         <v>13.104116928556801</v>
       </c>
-      <c r="J4" s="5">
+      <c r="K4" s="6">
+        <v>13.2821962536022</v>
+      </c>
+      <c r="L4" s="5">
         <v>0.92500996265842395</v>
       </c>
-      <c r="K4">
+      <c r="M4" s="9">
         <v>0.783376279585281</v>
       </c>
-      <c r="L4">
+      <c r="N4" s="9">
         <v>0.846160174782979</v>
       </c>
-      <c r="M4" s="6">
+      <c r="O4" s="9">
         <v>0.77556279443659204</v>
       </c>
-      <c r="N4" s="5">
+      <c r="P4" s="6">
+        <v>0.83843510215737604</v>
+      </c>
+      <c r="Q4" s="5">
         <v>3.12913192897709</v>
       </c>
-      <c r="O4">
+      <c r="R4" s="9">
         <v>7.2689280500914997</v>
       </c>
-      <c r="P4">
+      <c r="S4" s="9">
         <v>11.5473663195752</v>
       </c>
-      <c r="Q4" s="6">
+      <c r="T4" s="9">
         <v>13.109694372307899</v>
       </c>
-      <c r="R4" s="5">
+      <c r="U4" s="6">
+        <v>13.2821962536022</v>
+      </c>
+      <c r="V4" s="5">
         <v>0.26733949780492799</v>
       </c>
-      <c r="S4">
+      <c r="W4" s="9">
         <v>0.16366515737342499</v>
       </c>
-      <c r="T4">
+      <c r="X4" s="9">
         <v>0.668822149486343</v>
       </c>
-      <c r="U4" s="6">
+      <c r="Y4" s="9">
         <v>0.76998535068551099</v>
       </c>
+      <c r="Z4" s="6">
+        <v>0.83843510215737604</v>
+      </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A5">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A5" s="12">
         <f>10^5</f>
         <v>100000</v>
       </c>
       <c r="B5" s="5">
         <v>3.7476012874622202</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="9">
         <v>8.3297381635610002</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="9">
         <v>13.382716664078099</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="9">
         <v>16.084765993144899</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="6">
+        <v>16.583078683256598</v>
+      </c>
+      <c r="G5" s="5">
         <v>2.46641083389519</v>
       </c>
-      <c r="G5">
+      <c r="H5" s="9">
         <v>6.6706276155666098</v>
       </c>
-      <c r="H5">
+      <c r="I5" s="9">
         <v>12.299583176056201</v>
       </c>
-      <c r="I5" s="6">
+      <c r="J5" s="9">
         <v>15.954004985467</v>
       </c>
-      <c r="J5" s="5">
+      <c r="K5" s="6">
+        <v>16.578922106395801</v>
+      </c>
+      <c r="L5" s="5">
         <v>0.92107696590821697</v>
       </c>
-      <c r="K5">
+      <c r="M5" s="9">
         <v>0.77394504742076597</v>
       </c>
-      <c r="L5">
+      <c r="N5" s="9">
         <v>0.85386541048586395</v>
       </c>
-      <c r="M5" s="6">
+      <c r="O5" s="9">
         <v>0.77813330931064995</v>
       </c>
-      <c r="N5" s="5">
+      <c r="P5" s="6">
+        <v>0.837199648858166</v>
+      </c>
+      <c r="Q5" s="5">
         <v>3.1157223585129001</v>
       </c>
-      <c r="O5">
+      <c r="R5" s="9">
         <v>7.30852381426919</v>
       </c>
-      <c r="P5">
+      <c r="S5" s="9">
         <v>12.7290957882296</v>
       </c>
-      <c r="Q5" s="6">
+      <c r="T5" s="9">
         <v>15.9860086265292</v>
       </c>
-      <c r="R5" s="5">
+      <c r="U5" s="6">
+        <v>16.579329655270801</v>
+      </c>
+      <c r="V5" s="5">
         <v>0.27176544129049901</v>
       </c>
-      <c r="S5">
+      <c r="W5" s="9">
         <v>0.13604884871818601</v>
       </c>
-      <c r="T5">
+      <c r="X5" s="9">
         <v>0.42435279831242401</v>
       </c>
-      <c r="U5" s="6">
+      <c r="Y5" s="9">
         <v>0.74612966824844296</v>
       </c>
+      <c r="Z5" s="6">
+        <v>0.83679209998314197</v>
+      </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A6">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A6" s="12">
         <f>10^6</f>
         <v>1000000</v>
       </c>
       <c r="B6" s="5">
         <v>3.7465152996415299</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="9">
         <v>8.4182400250552103</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="9">
         <v>14.286303589658401</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="9">
         <v>18.597743295329</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="6">
+        <v>19.8254436337767</v>
+      </c>
+      <c r="G6" s="5">
         <v>2.4651018335014001</v>
       </c>
-      <c r="G6">
+      <c r="H6" s="9">
         <v>6.6735455139029698</v>
       </c>
-      <c r="H6">
+      <c r="I6" s="9">
         <v>12.496048018768199</v>
       </c>
-      <c r="I6" s="6">
+      <c r="J6" s="9">
         <v>18.142783746791899</v>
       </c>
-      <c r="J6" s="5">
+      <c r="K6" s="6">
+        <v>19.799628738701799</v>
+      </c>
+      <c r="L6" s="5">
         <v>0.92240723478879805</v>
       </c>
-      <c r="K6">
+      <c r="M6" s="9">
         <v>0.77244952593230498</v>
       </c>
-      <c r="L6">
+      <c r="N6" s="9">
         <v>0.85287101069609705</v>
       </c>
-      <c r="M6" s="6">
+      <c r="O6" s="9">
         <v>0.77728017706173003</v>
       </c>
-      <c r="N6" s="5">
+      <c r="P6" s="6">
+        <v>0.83800692990018699</v>
+      </c>
+      <c r="Q6" s="5">
         <v>3.1138931147827602</v>
       </c>
-      <c r="O6">
+      <c r="R6" s="9">
         <v>7.3106699747613302</v>
       </c>
-      <c r="P6">
+      <c r="S6" s="9">
         <v>13.0626440312352</v>
       </c>
-      <c r="Q6" s="6">
+      <c r="T6" s="9">
         <v>18.274602243557201</v>
       </c>
-      <c r="R6" s="5">
+      <c r="U6" s="6">
+        <v>19.801754088535599</v>
+      </c>
+      <c r="V6" s="5">
         <v>0.273615953507439</v>
       </c>
-      <c r="S6">
+      <c r="W6" s="9">
         <v>0.13532506507394701</v>
       </c>
-      <c r="T6">
+      <c r="X6" s="9">
         <v>0.28627499822907598</v>
       </c>
-      <c r="U6" s="6">
+      <c r="Y6" s="9">
         <v>0.64546168029639195</v>
       </c>
+      <c r="Z6" s="6">
+        <v>0.83588158006639501</v>
+      </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A7">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A7" s="12">
         <f>10^7</f>
         <v>10000000</v>
       </c>
       <c r="B7" s="5">
         <v>3.7534593168413699</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="9">
         <v>8.4351903362329992</v>
       </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="5">
+      <c r="D7" s="9">
+        <v>14.731522078548499</v>
+      </c>
+      <c r="E7" s="9">
+        <v>20.528859737092599</v>
+      </c>
+      <c r="F7" s="6"/>
+      <c r="G7" s="5">
         <v>2.4670473175865801</v>
       </c>
-      <c r="G7">
+      <c r="H7" s="9">
         <v>6.6719010781448498</v>
       </c>
-      <c r="I7" s="6"/>
-      <c r="J7" s="5">
+      <c r="I7" s="9">
+        <v>12.5167533640266</v>
+      </c>
+      <c r="J7" s="9">
+        <v>19.428817957621099</v>
+      </c>
+      <c r="K7" s="6"/>
+      <c r="L7" s="5">
         <v>0.92295228147605402</v>
       </c>
-      <c r="K7">
+      <c r="M7" s="9">
         <v>0.77108128921530195</v>
       </c>
-      <c r="M7" s="6"/>
-      <c r="N7" s="5">
+      <c r="N7" s="9">
+        <v>0.85310360314501399</v>
+      </c>
+      <c r="O7" s="9">
+        <v>0.77641459044955297</v>
+      </c>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="5">
         <v>3.1172502262584798</v>
       </c>
-      <c r="O7">
+      <c r="R7" s="9">
         <v>7.3078514469429301</v>
       </c>
-      <c r="Q7" s="6"/>
-      <c r="R7" s="5">
+      <c r="S7" s="9">
+        <v>13.1060836470333</v>
+      </c>
+      <c r="T7" s="9">
+        <v>19.7564424262657</v>
+      </c>
+      <c r="U7" s="6"/>
+      <c r="V7" s="5">
         <v>0.27274937280415701</v>
       </c>
-      <c r="S7">
+      <c r="W7" s="9">
         <v>0.13513092041722999</v>
       </c>
-      <c r="U7" s="6"/>
+      <c r="X7" s="9">
+        <v>0.26377332013827498</v>
+      </c>
+      <c r="Y7" s="9">
+        <v>0.44879012180496802</v>
+      </c>
+      <c r="Z7" s="6"/>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="7">
-        <f>2*2^2 * A11</f>
+        <f>2*2^2 * A13</f>
         <v>3.751964748714248</v>
       </c>
       <c r="C8" s="8">
-        <f>2*3^2 * A11</f>
+        <f>2*3^2 * A13</f>
         <v>8.4419206846070587</v>
       </c>
       <c r="D8" s="8">
-        <f>2*4^2 * A11</f>
+        <f>2*4^2 * A13</f>
         <v>15.007858994856992</v>
       </c>
-      <c r="E8" s="9">
-        <f>2*5^2 * A11</f>
+      <c r="E8" s="8">
+        <f>2*5^2 * A13</f>
         <v>23.449779679464051</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="8">
+        <f>2*6^2 * A13</f>
+        <v>33.767682738428235</v>
+      </c>
+      <c r="G8" s="7">
         <v>2.4669456687779099</v>
       </c>
-      <c r="G8" s="8">
+      <c r="H8" s="8">
         <v>6.67220940121718</v>
       </c>
-      <c r="H8" s="8"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="7">
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="7">
         <v>0.92286093473603703</v>
       </c>
-      <c r="K8" s="8">
+      <c r="M8" s="8">
         <v>0.771486086205461</v>
       </c>
-      <c r="L8" s="8"/>
-      <c r="M8" s="9"/>
-      <c r="N8" s="7">
+      <c r="N8" s="8"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="11"/>
+      <c r="Q8" s="7">
         <v>3.11677575940231</v>
       </c>
-      <c r="O8" s="8">
+      <c r="R8" s="8">
         <v>7.30867595446911</v>
       </c>
-      <c r="P8" s="8"/>
-      <c r="Q8" s="9"/>
-      <c r="R8" s="7">
+      <c r="S8" s="8"/>
+      <c r="T8" s="8"/>
+      <c r="U8" s="11"/>
+      <c r="V8" s="7">
         <v>0.27303084411163397</v>
       </c>
-      <c r="S8" s="8">
+      <c r="W8" s="8">
         <v>0.135019532953535</v>
       </c>
-      <c r="T8" s="8"/>
-      <c r="U8" s="9"/>
+      <c r="X8" s="8"/>
+      <c r="Y8" s="8"/>
+      <c r="Z8" s="11"/>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10">
+        <f>2^(2*(2^2))</f>
+        <v>256</v>
+      </c>
+      <c r="C10" s="12">
+        <f>2^(2*(3^2))</f>
+        <v>262144</v>
+      </c>
+      <c r="D10" s="12">
+        <f>2^(2*(4^2))</f>
+        <v>4294967296</v>
+      </c>
+      <c r="E10" s="12">
+        <f>2^(2*(5^2))</f>
+        <v>1125899906842624</v>
+      </c>
+      <c r="F10" s="12">
+        <f>2^(2*(6^2))</f>
+        <v>4.7223664828696452E+21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A11">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A13">
         <f>-0.1*IMLOG2(0.1)-0.9*IMLOG2(0.9)</f>
         <v>0.468995593589281</v>
       </c>

</xml_diff>

<commit_message>
Larger iterations of Monte Carlo for larger lattice size
It might become infeasible to simulate mutual information.
</commit_message>
<xml_diff>
--- a/Convergence.xlsx
+++ b/Convergence.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e00c848d2da39f20/Documents/3.Masters/Thesis/Code/MutualInfo/QEC_MI_MonteCarlo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e00c848d2da39f20/Documents/3. Masters/Thesis/Code/MutualInfo/QEC_MI_MonteCarlo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="332" documentId="11_F25DC773A252ABDACC1048BDC11F63425BDE58E3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{05388BDA-CB1E-43DD-A7A6-CCEECD11FB15}"/>
+  <xr:revisionPtr revIDLastSave="351" documentId="11_F25DC773A252ABDACC1048BDC11F63425BDE58E3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{36CF9C8E-6026-465C-B5CD-C7FEC1F152AE}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -201,7 +201,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -211,8 +211,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
@@ -1097,15 +1095,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>396240</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>156210</xdr:rowOff>
+      <xdr:colOff>613955</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>47353</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>91440</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>156210</xdr:rowOff>
+      <xdr:colOff>309155</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>47352</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1400,10 +1398,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z13"/>
+  <dimension ref="A1:Z15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1457,73 +1455,73 @@
       <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="6" t="s">
         <v>12</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="J2" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="10" t="s">
+      <c r="K2" s="6" t="s">
         <v>12</v>
       </c>
       <c r="L2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="M2" s="9" t="s">
+      <c r="M2" t="s">
         <v>1</v>
       </c>
-      <c r="N2" s="9" t="s">
+      <c r="N2" t="s">
         <v>2</v>
       </c>
-      <c r="O2" s="9" t="s">
+      <c r="O2" t="s">
         <v>11</v>
       </c>
-      <c r="P2" s="10" t="s">
+      <c r="P2" s="6" t="s">
         <v>12</v>
       </c>
       <c r="Q2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="R2" s="9" t="s">
+      <c r="R2" t="s">
         <v>1</v>
       </c>
-      <c r="S2" s="9" t="s">
+      <c r="S2" t="s">
         <v>2</v>
       </c>
-      <c r="T2" s="9" t="s">
+      <c r="T2" t="s">
         <v>11</v>
       </c>
-      <c r="U2" s="10" t="s">
+      <c r="U2" s="6" t="s">
         <v>12</v>
       </c>
       <c r="V2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="W2" s="9" t="s">
+      <c r="W2" t="s">
         <v>1</v>
       </c>
-      <c r="X2" s="9" t="s">
+      <c r="X2" t="s">
         <v>2</v>
       </c>
-      <c r="Y2" s="9" t="s">
+      <c r="Y2" t="s">
         <v>11</v>
       </c>
       <c r="Z2" s="6" t="s">
@@ -1531,20 +1529,20 @@
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A3" s="12">
+      <c r="A3" s="10">
         <f>10^3</f>
         <v>1000</v>
       </c>
       <c r="B3" s="5">
         <v>3.63906932787524</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3">
         <v>7.35273934818116</v>
       </c>
-      <c r="D3" s="9">
+      <c r="D3">
         <v>9.5504002180521397</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E3">
         <v>9.9242745096576908</v>
       </c>
       <c r="F3" s="6">
@@ -1553,13 +1551,13 @@
       <c r="G3" s="5">
         <v>2.4472065907296798</v>
       </c>
-      <c r="H3" s="9">
+      <c r="H3">
         <v>6.6309771114962697</v>
       </c>
-      <c r="I3" s="9">
+      <c r="I3">
         <v>9.4651160055370003</v>
       </c>
-      <c r="J3" s="9">
+      <c r="J3">
         <v>9.9242745096576908</v>
       </c>
       <c r="K3" s="6">
@@ -1568,13 +1566,13 @@
       <c r="L3" s="5">
         <v>0.93317179842408904</v>
       </c>
-      <c r="M3" s="9">
+      <c r="M3">
         <v>0.75093197963384595</v>
       </c>
-      <c r="N3" s="9">
+      <c r="N3">
         <v>0.86872124633940395</v>
       </c>
-      <c r="O3" s="9">
+      <c r="O3">
         <v>0.783204430282889</v>
       </c>
       <c r="P3" s="6">
@@ -1583,13 +1581,13 @@
       <c r="Q3" s="5">
         <v>3.0503907781573201</v>
       </c>
-      <c r="R3" s="9">
+      <c r="R3">
         <v>7.0390890884613802</v>
       </c>
-      <c r="S3" s="9">
+      <c r="S3">
         <v>9.5001355555456506</v>
       </c>
-      <c r="T3" s="9">
+      <c r="T3">
         <v>9.9242745096576908</v>
       </c>
       <c r="U3" s="6">
@@ -1598,13 +1596,13 @@
       <c r="V3" s="5">
         <v>0.32998761099645002</v>
       </c>
-      <c r="W3" s="9">
+      <c r="W3">
         <v>0.34282000266873702</v>
       </c>
-      <c r="X3" s="9">
+      <c r="X3">
         <v>0.83370169633075197</v>
       </c>
-      <c r="Y3" s="9">
+      <c r="Y3">
         <v>0.783204430282889</v>
       </c>
       <c r="Z3" s="6">
@@ -1612,20 +1610,20 @@
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A4" s="12">
+      <c r="A4" s="10">
         <f>10^4</f>
         <v>10000</v>
       </c>
       <c r="B4" s="5">
         <v>3.7649003376452002</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4">
         <v>8.0198059704979006</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4">
         <v>11.7721183211632</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4">
         <v>13.128361893507099</v>
       </c>
       <c r="F4" s="6">
@@ -1634,13 +1632,13 @@
       <c r="G4" s="5">
         <v>2.4714614641235899</v>
       </c>
-      <c r="H4" s="9">
+      <c r="H4">
         <v>6.6492169278796398</v>
       </c>
-      <c r="I4" s="9">
+      <c r="I4">
         <v>11.3700282942785</v>
       </c>
-      <c r="J4" s="9">
+      <c r="J4">
         <v>13.104116928556801</v>
       </c>
       <c r="K4" s="6">
@@ -1649,13 +1647,13 @@
       <c r="L4" s="5">
         <v>0.92500996265842395</v>
       </c>
-      <c r="M4" s="9">
+      <c r="M4">
         <v>0.783376279585281</v>
       </c>
-      <c r="N4" s="9">
+      <c r="N4">
         <v>0.846160174782979</v>
       </c>
-      <c r="O4" s="9">
+      <c r="O4">
         <v>0.77556279443659204</v>
       </c>
       <c r="P4" s="6">
@@ -1664,13 +1662,13 @@
       <c r="Q4" s="5">
         <v>3.12913192897709</v>
       </c>
-      <c r="R4" s="9">
+      <c r="R4">
         <v>7.2689280500914997</v>
       </c>
-      <c r="S4" s="9">
+      <c r="S4">
         <v>11.5473663195752</v>
       </c>
-      <c r="T4" s="9">
+      <c r="T4">
         <v>13.109694372307899</v>
       </c>
       <c r="U4" s="6">
@@ -1679,13 +1677,13 @@
       <c r="V4" s="5">
         <v>0.26733949780492799</v>
       </c>
-      <c r="W4" s="9">
+      <c r="W4">
         <v>0.16366515737342499</v>
       </c>
-      <c r="X4" s="9">
+      <c r="X4">
         <v>0.668822149486343</v>
       </c>
-      <c r="Y4" s="9">
+      <c r="Y4">
         <v>0.76998535068551099</v>
       </c>
       <c r="Z4" s="6">
@@ -1693,20 +1691,20 @@
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A5" s="12">
+      <c r="A5" s="10">
         <f>10^5</f>
         <v>100000</v>
       </c>
       <c r="B5" s="5">
         <v>3.7476012874622202</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5">
         <v>8.3297381635610002</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5">
         <v>13.382716664078099</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5">
         <v>16.084765993144899</v>
       </c>
       <c r="F5" s="6">
@@ -1715,13 +1713,13 @@
       <c r="G5" s="5">
         <v>2.46641083389519</v>
       </c>
-      <c r="H5" s="9">
+      <c r="H5">
         <v>6.6706276155666098</v>
       </c>
-      <c r="I5" s="9">
+      <c r="I5">
         <v>12.299583176056201</v>
       </c>
-      <c r="J5" s="9">
+      <c r="J5">
         <v>15.954004985467</v>
       </c>
       <c r="K5" s="6">
@@ -1730,13 +1728,13 @@
       <c r="L5" s="5">
         <v>0.92107696590821697</v>
       </c>
-      <c r="M5" s="9">
+      <c r="M5">
         <v>0.77394504742076597</v>
       </c>
-      <c r="N5" s="9">
+      <c r="N5">
         <v>0.85386541048586395</v>
       </c>
-      <c r="O5" s="9">
+      <c r="O5">
         <v>0.77813330931064995</v>
       </c>
       <c r="P5" s="6">
@@ -1745,13 +1743,13 @@
       <c r="Q5" s="5">
         <v>3.1157223585129001</v>
       </c>
-      <c r="R5" s="9">
+      <c r="R5">
         <v>7.30852381426919</v>
       </c>
-      <c r="S5" s="9">
+      <c r="S5">
         <v>12.7290957882296</v>
       </c>
-      <c r="T5" s="9">
+      <c r="T5">
         <v>15.9860086265292</v>
       </c>
       <c r="U5" s="6">
@@ -1760,13 +1758,13 @@
       <c r="V5" s="5">
         <v>0.27176544129049901</v>
       </c>
-      <c r="W5" s="9">
+      <c r="W5">
         <v>0.13604884871818601</v>
       </c>
-      <c r="X5" s="9">
+      <c r="X5">
         <v>0.42435279831242401</v>
       </c>
-      <c r="Y5" s="9">
+      <c r="Y5">
         <v>0.74612966824844296</v>
       </c>
       <c r="Z5" s="6">
@@ -1774,20 +1772,20 @@
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A6" s="12">
+      <c r="A6" s="10">
         <f>10^6</f>
         <v>1000000</v>
       </c>
       <c r="B6" s="5">
         <v>3.7465152996415299</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6">
         <v>8.4182400250552103</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6">
         <v>14.286303589658401</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6">
         <v>18.597743295329</v>
       </c>
       <c r="F6" s="6">
@@ -1796,13 +1794,13 @@
       <c r="G6" s="5">
         <v>2.4651018335014001</v>
       </c>
-      <c r="H6" s="9">
+      <c r="H6">
         <v>6.6735455139029698</v>
       </c>
-      <c r="I6" s="9">
+      <c r="I6">
         <v>12.496048018768199</v>
       </c>
-      <c r="J6" s="9">
+      <c r="J6">
         <v>18.142783746791899</v>
       </c>
       <c r="K6" s="6">
@@ -1811,13 +1809,13 @@
       <c r="L6" s="5">
         <v>0.92240723478879805</v>
       </c>
-      <c r="M6" s="9">
+      <c r="M6">
         <v>0.77244952593230498</v>
       </c>
-      <c r="N6" s="9">
+      <c r="N6">
         <v>0.85287101069609705</v>
       </c>
-      <c r="O6" s="9">
+      <c r="O6">
         <v>0.77728017706173003</v>
       </c>
       <c r="P6" s="6">
@@ -1826,13 +1824,13 @@
       <c r="Q6" s="5">
         <v>3.1138931147827602</v>
       </c>
-      <c r="R6" s="9">
+      <c r="R6">
         <v>7.3106699747613302</v>
       </c>
-      <c r="S6" s="9">
+      <c r="S6">
         <v>13.0626440312352</v>
       </c>
-      <c r="T6" s="9">
+      <c r="T6">
         <v>18.274602243557201</v>
       </c>
       <c r="U6" s="6">
@@ -1841,13 +1839,13 @@
       <c r="V6" s="5">
         <v>0.273615953507439</v>
       </c>
-      <c r="W6" s="9">
+      <c r="W6">
         <v>0.13532506507394701</v>
       </c>
-      <c r="X6" s="9">
+      <c r="X6">
         <v>0.28627499822907598</v>
       </c>
-      <c r="Y6" s="9">
+      <c r="Y6">
         <v>0.64546168029639195</v>
       </c>
       <c r="Z6" s="6">
@@ -1855,169 +1853,189 @@
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A7" s="12">
+      <c r="A7" s="10">
         <f>10^7</f>
         <v>10000000</v>
       </c>
       <c r="B7" s="5">
         <v>3.7534593168413699</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7">
         <v>8.4351903362329992</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7">
         <v>14.731522078548499</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7">
         <v>20.528859737092599</v>
       </c>
-      <c r="F7" s="6"/>
+      <c r="F7" s="6">
+        <v>22.928278335105901</v>
+      </c>
       <c r="G7" s="5">
         <v>2.4670473175865801</v>
       </c>
-      <c r="H7" s="9">
+      <c r="H7">
         <v>6.6719010781448498</v>
       </c>
-      <c r="I7" s="9">
+      <c r="I7">
         <v>12.5167533640266</v>
       </c>
-      <c r="J7" s="9">
+      <c r="J7">
         <v>19.428817957621099</v>
       </c>
-      <c r="K7" s="6"/>
+      <c r="K7" s="6">
+        <v>22.820774259042</v>
+      </c>
       <c r="L7" s="5">
         <v>0.92295228147605402</v>
       </c>
-      <c r="M7" s="9">
+      <c r="M7">
         <v>0.77108128921530195</v>
       </c>
-      <c r="N7" s="9">
+      <c r="N7">
         <v>0.85310360314501399</v>
       </c>
-      <c r="O7" s="9">
+      <c r="O7">
         <v>0.77641459044955297</v>
       </c>
-      <c r="P7" s="6"/>
+      <c r="P7" s="6">
+        <v>0.83716017215875405</v>
+      </c>
       <c r="Q7" s="5">
         <v>3.1172502262584798</v>
       </c>
-      <c r="R7" s="9">
+      <c r="R7">
         <v>7.3078514469429301</v>
       </c>
-      <c r="S7" s="9">
+      <c r="S7">
         <v>13.1060836470333</v>
       </c>
-      <c r="T7" s="9">
+      <c r="T7">
         <v>19.7564424262657</v>
       </c>
-      <c r="U7" s="6"/>
+      <c r="U7" s="6">
+        <v>22.8337258456556</v>
+      </c>
       <c r="V7" s="5">
         <v>0.27274937280415701</v>
       </c>
-      <c r="W7" s="9">
+      <c r="W7">
         <v>0.13513092041722999</v>
       </c>
-      <c r="X7" s="9">
+      <c r="X7">
         <v>0.26377332013827498</v>
       </c>
-      <c r="Y7" s="9">
+      <c r="Y7">
         <v>0.44879012180496802</v>
       </c>
-      <c r="Z7" s="6"/>
+      <c r="Z7" s="6">
+        <v>0.82420858554516396</v>
+      </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="7">
-        <f>2*2^2 * A13</f>
-        <v>3.751964748714248</v>
-      </c>
-      <c r="C8" s="8">
-        <f>2*3^2 * A13</f>
-        <v>8.4419206846070587</v>
-      </c>
-      <c r="D8" s="8">
-        <f>2*4^2 * A13</f>
-        <v>15.007858994856992</v>
-      </c>
-      <c r="E8" s="8">
-        <f>2*5^2 * A13</f>
-        <v>23.449779679464051</v>
-      </c>
-      <c r="F8" s="8">
-        <f>2*6^2 * A13</f>
-        <v>33.767682738428235</v>
-      </c>
-      <c r="G8" s="7">
-        <v>2.4669456687779099</v>
-      </c>
-      <c r="H8" s="8">
-        <v>6.67220940121718</v>
-      </c>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="11"/>
-      <c r="L8" s="7">
-        <v>0.92286093473603703</v>
-      </c>
-      <c r="M8" s="8">
-        <v>0.771486086205461</v>
-      </c>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8"/>
-      <c r="P8" s="11"/>
-      <c r="Q8" s="7">
-        <v>3.11677575940231</v>
-      </c>
-      <c r="R8" s="8">
-        <v>7.30867595446911</v>
-      </c>
-      <c r="S8" s="8"/>
-      <c r="T8" s="8"/>
-      <c r="U8" s="11"/>
-      <c r="V8" s="7">
-        <v>0.27303084411163397</v>
-      </c>
-      <c r="W8" s="8">
-        <v>0.135019532953535</v>
-      </c>
-      <c r="X8" s="8"/>
-      <c r="Y8" s="8"/>
-      <c r="Z8" s="11"/>
+      <c r="A8" s="10">
+        <v>100000000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A9" s="10">
+        <v>1000000000</v>
+      </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10">
-        <f>2^(2*(2^2))</f>
-        <v>256</v>
-      </c>
-      <c r="C10" s="12">
-        <f>2^(2*(3^2))</f>
-        <v>262144</v>
-      </c>
-      <c r="D10" s="12">
-        <f>2^(2*(4^2))</f>
-        <v>4294967296</v>
-      </c>
-      <c r="E10" s="12">
-        <f>2^(2*(5^2))</f>
-        <v>1125899906842624</v>
-      </c>
-      <c r="F10" s="12">
-        <f>2^(2*(6^2))</f>
-        <v>4.7223664828696452E+21</v>
-      </c>
+      <c r="A10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="7">
+        <f>2*2^2 * A15</f>
+        <v>3.751964748714248</v>
+      </c>
+      <c r="C10" s="8">
+        <f>2*3^2 * A15</f>
+        <v>8.4419206846070587</v>
+      </c>
+      <c r="D10" s="8">
+        <f>2*4^2 * A15</f>
+        <v>15.007858994856992</v>
+      </c>
+      <c r="E10" s="8">
+        <f>2*5^2 * A15</f>
+        <v>23.449779679464051</v>
+      </c>
+      <c r="F10" s="8">
+        <f>2*6^2 * A15</f>
+        <v>33.767682738428235</v>
+      </c>
+      <c r="G10" s="7">
+        <v>2.4669456687779099</v>
+      </c>
+      <c r="H10" s="8">
+        <v>6.67220940121718</v>
+      </c>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="7">
+        <v>0.92286093473603703</v>
+      </c>
+      <c r="M10" s="8">
+        <v>0.771486086205461</v>
+      </c>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="9"/>
+      <c r="Q10" s="7">
+        <v>3.11677575940231</v>
+      </c>
+      <c r="R10" s="8">
+        <v>7.30867595446911</v>
+      </c>
+      <c r="S10" s="8"/>
+      <c r="T10" s="8"/>
+      <c r="U10" s="9"/>
+      <c r="V10" s="7">
+        <v>0.27303084411163397</v>
+      </c>
+      <c r="W10" s="8">
+        <v>0.135019532953535</v>
+      </c>
+      <c r="X10" s="8"/>
+      <c r="Y10" s="8"/>
+      <c r="Z10" s="9"/>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12">
+        <f>2^(2*(2^2))</f>
+        <v>256</v>
+      </c>
+      <c r="C12" s="10">
+        <f>2^(2*(3^2))</f>
+        <v>262144</v>
+      </c>
+      <c r="D12" s="10">
+        <f>2^(2*(4^2))</f>
+        <v>4294967296</v>
+      </c>
+      <c r="E12" s="10">
+        <f>2^(2*(5^2))</f>
+        <v>1125899906842624</v>
+      </c>
+      <c r="F12" s="10">
+        <f>2^(2*(6^2))</f>
+        <v>4.7223664828696452E+21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A13">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A15">
         <f>-0.1*IMLOG2(0.1)-0.9*IMLOG2(0.9)</f>
         <v>0.468995593589281</v>
       </c>

</xml_diff>

<commit_message>
New method to estimate MI
We approximate the binomial distribution as a Gaussian for number of errors occurring, and then analyze the probability distributions of H(S), H(EC), H(S,EC) for number of errors of 0 up to mu+x sigma for some x. This can significantly reduce the run-time but should still be exponential in L.
</commit_message>
<xml_diff>
--- a/Convergence.xlsx
+++ b/Convergence.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e00c848d2da39f20/Documents/3. Masters/Thesis/Code/MutualInfo/QEC_MI_MonteCarlo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="525" documentId="11_F25DC773A252ABDACC1048BDC11F63425BDE58E3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F27276FE-C4F3-4338-90AC-E83995F399A4}"/>
+  <xr:revisionPtr revIDLastSave="532" documentId="11_F25DC773A252ABDACC1048BDC11F63425BDE58E3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{39296F83-7D42-4AF6-931C-086F61500651}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -548,8 +548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V15" sqref="V15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1088,17 +1088,32 @@
       <c r="D8">
         <v>14.9151373071108</v>
       </c>
+      <c r="E8">
+        <v>21.8581528274173</v>
+      </c>
       <c r="I8">
         <v>12.518538685125099</v>
       </c>
+      <c r="J8">
+        <v>19.915534863938198</v>
+      </c>
       <c r="N8">
         <v>0.85269273426893299</v>
       </c>
+      <c r="O8">
+        <v>0.776759928225073</v>
+      </c>
       <c r="S8">
         <v>13.109603870236199</v>
       </c>
+      <c r="T8">
+        <v>20.426284399082501</v>
+      </c>
       <c r="X8">
         <v>0.26162754915785502</v>
+      </c>
+      <c r="Y8">
+        <v>0.26601039308078001</v>
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
We now use the PYM entropy estimator to compute
See https://github.com/pillowlab/PYMentropy
</commit_message>
<xml_diff>
--- a/Convergence.xlsx
+++ b/Convergence.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e00c848d2da39f20/Documents/3. Masters/Thesis/Code/MutualInfo/QEC_MI_MonteCarlo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="532" documentId="11_F25DC773A252ABDACC1048BDC11F63425BDE58E3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{39296F83-7D42-4AF6-931C-086F61500651}"/>
+  <xr:revisionPtr revIDLastSave="536" documentId="11_F25DC773A252ABDACC1048BDC11F63425BDE58E3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F06DBFF2-82DF-4A74-9E61-D4987E7D4DFC}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -277,6 +277,908 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:strRef>
+              <c:f>(Sheet1!$G$2,Sheet1!$I$2,Sheet1!$K$2)</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>L=2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>L=4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>L=6</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(Sheet1!$G$7,Sheet1!$I$8,Sheet1!$K$7)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2.4670473175865801</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12.518538685125099</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22.820774259042</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C522-4F10-B777-0C596376D0C3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1994661679"/>
+        <c:axId val="1994662159"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1994661679"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1994662159"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1994662159"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1994661679"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>119429</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>69361</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>419345</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>50312</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{461BBFA8-AE7C-D62B-1EAB-D1B205E920E6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
@@ -548,18 +1450,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V15" sqref="V15"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="T24" sqref="T24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.453125" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
@@ -596,7 +1498,7 @@
       <c r="Y1" s="3"/>
       <c r="Z1" s="4"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -676,7 +1578,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A3" s="10">
         <f>10^3</f>
         <v>1000</v>
@@ -757,7 +1659,7 @@
         <v>0.87129078401035898</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A4" s="10">
         <f>10^4</f>
         <v>10000</v>
@@ -838,7 +1740,7 @@
         <v>0.83843510215737604</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A5" s="10">
         <f>10^5</f>
         <v>100000</v>
@@ -919,7 +1821,7 @@
         <v>0.83679209998314197</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A6" s="10">
         <f>10^6</f>
         <v>1000000</v>
@@ -1000,7 +1902,7 @@
         <v>0.83588158006639501</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A7" s="10">
         <f>10^7</f>
         <v>10000000</v>
@@ -1081,7 +1983,7 @@
         <v>0.82420858554516396</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A8" s="10">
         <v>100000000</v>
       </c>
@@ -1116,12 +2018,12 @@
         <v>0.26601039308078001</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A9" s="10">
         <v>1000000000</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>3</v>
       </c>
@@ -1182,7 +2084,7 @@
       <c r="Y10" s="8"/>
       <c r="Z10" s="9"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -1207,12 +2109,12 @@
         <v>4.7223664828696452E+21</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A15">
         <f>-0.1*IMLOG2(0.1)-0.9*IMLOG2(0.9)</f>
         <v>0.468995593589281</v>
@@ -1224,7 +2126,7 @@
         <v>1.53</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.35">
       <c r="D16" t="s">
         <v>18</v>
       </c>
@@ -1232,7 +2134,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
       <c r="D17" t="s">
         <v>19</v>
       </c>
@@ -1240,7 +2142,7 @@
         <v>0.1028</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -1269,7 +2171,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>3</v>
       </c>
@@ -1312,7 +2214,7 @@
         <v>-11.365035022041235</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>5</v>
       </c>
@@ -1353,7 +2255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
       <c r="K21">
         <v>1</v>
       </c>
@@ -1367,7 +2269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
       <c r="K22" t="e">
         <v>#NUM!</v>
       </c>
@@ -1381,7 +2283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
       <c r="K23">
         <v>81.369464134933025</v>
       </c>
@@ -1398,5 +2300,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>